<commit_message>
Added some changes to allow easier running of programs
</commit_message>
<xml_diff>
--- a/results/roundabout_full.txt_50_ce_err.xlsx
+++ b/results/roundabout_full.txt_50_ce_err.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artyom\Documents\Projects\autonomous_vehicles1\path-planning-simulation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8C4D12-34AD-4CD7-93B0-97871F1A0A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517C31AB-ABCF-470E-973E-FFE2302A3D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="roundabout_full.txt_50_ce_err" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>Stanley with lookahead</t>
   </si>
   <si>
-    <t>Hybrid Stanley and Pure Pursuit</t>
+    <t>Combined Stanley and Pure Pursuit</t>
   </si>
 </sst>
 </file>
@@ -699,7 +699,7 @@
                   <c:v>Stanley with lookahead</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Hybrid Stanley and Pure Pursuit</c:v>
+                  <c:v>Combined Stanley and Pure Pursuit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1896,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="O109" sqref="O109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="E123" t="str">
         <f t="shared" si="0"/>
-        <v>Hybrid Stanley and Pure Pursuit</v>
+        <v>Combined Stanley and Pure Pursuit</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>